<commit_message>
Moved from single string for the error report to a report object (in the syntaxreport package)
</commit_message>
<xml_diff>
--- a/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2021.syntax_checked.xlsx
+++ b/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2021.syntax_checked.xlsx
@@ -694,6 +694,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AEFSyntaxCheck</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Version' must conform to X.Y.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AEFSyntaxCheck</author>
+  </authors>
+  <commentList>
+    <comment ref="L8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Activity type(s)' can only contain alphanumeric, and space characters.</t>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Purposes for authorization' must be one of 'NDC', 'OIMP', 'IMP', 'OP', 'NDC and OIMP', 'NDC and IMP', or 'NDC and OP'.</t>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Authorized Party(ies) ID' must a comma-separated list of ISO 3166 alpha-3 codes.</t>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Authorized timeframe' must be empty of a year range (dddd - dddd)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AEFSyntaxCheck</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Action date must be in the format dd/mm/yyyy</t>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Action type'' must be one of 'Acquistion', 'Transfer', 'Use', 'Cancellation', 'First transfer'</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
+      </text>
+    </comment>
+    <comment ref="Y9" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AEFSyntaxCheck</author>
+  </authors>
+  <commentList>
+    <comment ref="D8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AEFSyntaxCheck</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0">
+      <text>
+        <t>Cell content error: The value provided for 'Date of the authorization must be in the format dd/mm/yyyy</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2329,6 +2444,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -2746,6 +2862,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -3379,6 +3496,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -4122,6 +4240,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -4249,6 +4368,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -4258,7 +4378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4269,37 +4389,335 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-	Correct number of worksheets in workbook.
-	All workseets found in workbook.
-	Checking the structure of 'Table 1 Submission'
-	Checking the structure of 'Table 2 Authorizations'
-	Checking the structure of 'Table 3 Actions'
-	Checking the structure of 'Table 4 Holdings'
-	Checking the structure of 'Table 5 Auth. entities'
-	Checking the content of 'Table 1 Submission'
-		Cell content error: The value provided for 'Version' must conform to X.Y.
-	Checking the content of 'Table 2 Authorizations'
-		Cell content error: The value provided for 'Activity type(s)' can only contain alphanumeric, and space characters.
-		Cell content error: The value provided for 'Purposes for authorization' must be one of 'NDC', 'OIMP', 'IMP', 'OP', 'NDC and OIMP', 'NDC and IMP', or 'NDC and OP'.
-		Cell content error: The value provided for 'Authorized Party(ies) ID' must a comma-separated list of ISO 3166 alpha-3 codes.
-		Cell content error: The value provided for 'Authorized timeframe' must be empty of a year range (dddd - dddd)
-	Checking the content of 'Table 3 Actions'
-		Cell content error: The value provided for 'Action date must be in the format dd/mm/yyyy
-		Cell content error: The value provided for 'Action type'' must be one of 'Acquistion', 'Transfer', 'Use', 'Cancellation', 'First transfer'
-		Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.
-		Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits
-		Cell content error: The value provided for 'Transferring participating Party ID' must an ISO 3166 alpha-3 country code.
-	Checking the content of 'Table 4 Holdings'
-		Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.
-		Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits
-	Checking the content of 'Table 5 Auth. entities'
-		Cell content error: The value provided for 'Date of the authorization must be in the format dd/mm/yyyy
-Syntax check found errors.</t>
+          <t>202504292100---AEF_CMA6_second_iteration - Guyana 2021.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Correct number of worksheets in workbook.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Index</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Summary information</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Table 1 Submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Table 2 Authorizations</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Table 3 Actions</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Table 4 Holdings</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Table 5 Auth. entities</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>All workseets found in workbook.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Summary information</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Table 1 Submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Table 2 Authorizations</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Table 3 Actions</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Table 4 Holdings</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Table 5 Auth. entities</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Checking the content of 'Table 1 Submission'</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Version' must conform to X.Y.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Checking the content of 'Table 2 Authorizations'</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Activity type(s)' can only contain alphanumeric, and space characters.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Purposes for authorization' must be one of 'NDC', 'OIMP', 'IMP', 'OP', 'NDC and OIMP', 'NDC and IMP', or 'NDC and OP'.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Authorized Party(ies) ID' must a comma-separated list of ISO 3166 alpha-3 codes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Authorized timeframe' must be empty of a year range (dddd - dddd)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Checking the content of 'Table 3 Actions'</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Action date must be in the format dd/mm/yyyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Action type'' must be one of 'Acquistion', 'Transfer', 'Use', 'Cancellation', 'First transfer'</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Checking the content of 'Table 4 Holdings'</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Checking the content of 'Table 5 Auth. entities'</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Cell content error: The value provided for 'Date of the authorization must be in the format dd/mm/yyyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Syntax check found errors.</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C22" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C23" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C24" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C25" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C27" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C28" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C29" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C30" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C31" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C33" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C34" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C36" r:id="rId13"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4616,17 +5034,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C842FC7A-C245-4356-AAD4-710BFFAA3AD1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD914F1E-4F53-45F4-BC1E-7EF3F88A5A0E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D01E7B4-526F-44B0-B126-705F785DCCEA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B1A0AE8-CC32-4283-A5C1-87C74821E965}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1AEA3B2-0ED9-4951-A8F2-4000B72EC836}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1590130-25C9-48B8-82F8-D67A90BF65B1}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A12CE63-201D-44DE-B00F-CBC7531629D9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5235138C-9377-42AF-9E7B-B62B08CD6318}"/>
 </file>
</xml_diff>

<commit_message>
Refactoring and output formatting changes
</commit_message>
<xml_diff>
--- a/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2021.syntax_checked.xlsx
+++ b/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2021.syntax_checked.xlsx
@@ -343,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -580,6 +580,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -601,20 +607,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -700,9 +694,9 @@
     <author>AEFSyntaxCheck</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>Cell content error: The value provided for 'Version' must conform to X.Y.</t>
+        <t>All fields found.</t>
       </text>
     </comment>
   </commentList>
@@ -715,24 +709,9 @@
     <author>AEFSyntaxCheck</author>
   </authors>
   <commentList>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>Cell content error: The value provided for 'Activity type(s)' can only contain alphanumeric, and space characters.</t>
-      </text>
-    </comment>
-    <comment ref="M8" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Purposes for authorization' must be one of 'NDC', 'OIMP', 'IMP', 'OP', 'NDC and OIMP', 'NDC and IMP', or 'NDC and OP'.</t>
-      </text>
-    </comment>
-    <comment ref="N8" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Authorized Party(ies) ID' must a comma-separated list of ISO 3166 alpha-3 codes.</t>
-      </text>
-    </comment>
-    <comment ref="Q8" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Authorized timeframe' must be empty of a year range (dddd - dddd)</t>
+        <t>All fields found.</t>
       </text>
     </comment>
   </commentList>
@@ -745,29 +724,9 @@
     <author>AEFSyntaxCheck</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>Cell content error: The value provided for 'Action date must be in the format dd/mm/yyyy</t>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Action type'' must be one of 'Acquistion', 'Transfer', 'Use', 'Cancellation', 'First transfer'</t>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
-      </text>
-    </comment>
-    <comment ref="Y9" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
+        <t>The field 'Authorized quantity' cannot be found in worksheet</t>
       </text>
     </comment>
   </commentList>
@@ -780,14 +739,9 @@
     <author>AEFSyntaxCheck</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
-      <text>
-        <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
+        <t>All fields found.</t>
       </text>
     </comment>
   </commentList>
@@ -800,9 +754,24 @@
     <author>AEFSyntaxCheck</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>Cell content error: The value provided for 'Date of the authorization must be in the format dd/mm/yyyy</t>
+        <t>All fields found.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AEFSyntaxCheck</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>All fields found.</t>
       </text>
     </comment>
   </commentList>
@@ -1213,7 +1182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C104"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView topLeftCell="A65" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C82" sqref="C82:C83"/>
@@ -1231,6 +1200,7 @@
   </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" t="n"/>
       <c r="B1" s="15" t="inlineStr">
         <is>
           <t> </t>
@@ -2305,6 +2275,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -2314,7 +2285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:C13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
@@ -2328,6 +2299,9 @@
     <col width="8.83203125" customWidth="1" style="1" min="4" max="16384"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n"/>
+    </row>
     <row r="3" ht="16" customHeight="1" thickBot="1">
       <c r="B3" s="6" t="inlineStr">
         <is>
@@ -2374,7 +2348,7 @@
           <t>Date of submission</t>
         </is>
       </c>
-      <c r="C7" s="101" t="n">
+      <c r="C7" s="92" t="n">
         <v>45904</v>
       </c>
     </row>
@@ -2435,8 +2409,8 @@
       </c>
     </row>
     <row r="13" ht="16" customHeight="1" thickTop="1">
-      <c r="B13" s="92" t="n"/>
-      <c r="C13" s="102" t="n"/>
+      <c r="B13" s="94" t="n"/>
+      <c r="C13" s="101" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2454,10 +2428,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:U14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2484,6 +2458,9 @@
     <col width="8.83203125" customWidth="1" style="15" min="22" max="16384"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n"/>
+    </row>
     <row r="3">
       <c r="B3" s="17" t="n"/>
     </row>
@@ -2495,14 +2472,14 @@
       </c>
     </row>
     <row r="5" ht="14.5" customHeight="1">
-      <c r="B5" s="93" t="inlineStr">
+      <c r="B5" s="95" t="inlineStr">
         <is>
           <t>Authorization</t>
         </is>
       </c>
-      <c r="C5" s="103" t="n"/>
-      <c r="D5" s="103" t="n"/>
-      <c r="E5" s="103" t="n"/>
+      <c r="C5" s="102" t="n"/>
+      <c r="D5" s="102" t="n"/>
+      <c r="E5" s="102" t="n"/>
       <c r="F5" s="33" t="n"/>
       <c r="G5" s="34" t="inlineStr">
         <is>
@@ -2570,7 +2547,7 @@
       <c r="F7" s="21" t="n"/>
       <c r="G7" s="21" t="inlineStr">
         <is>
-          <t>Authorized quantity</t>
+          <t>Authorized quantity2</t>
         </is>
       </c>
       <c r="H7" s="21" t="inlineStr">
@@ -2650,7 +2627,7 @@
           <t>GUY 2024-CA1</t>
         </is>
       </c>
-      <c r="C8" s="104" t="n">
+      <c r="C8" s="93" t="n">
         <v>45334</v>
       </c>
       <c r="D8" s="82" t="inlineStr">
@@ -2872,7 +2849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:AH13"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
@@ -2914,6 +2891,9 @@
     <col width="8.83203125" customWidth="1" style="15" min="33" max="16384"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n"/>
+    </row>
     <row r="3">
       <c r="B3" s="26" t="inlineStr">
         <is>
@@ -3047,21 +3027,21 @@
       <c r="V6" s="38" t="n"/>
       <c r="W6" s="38" t="n"/>
       <c r="X6" s="36" t="n"/>
-      <c r="Y6" s="95" t="inlineStr">
+      <c r="Y6" s="97" t="inlineStr">
         <is>
           <t xml:space="preserve"> Transfer / Acquisition</t>
         </is>
       </c>
-      <c r="Z6" s="103" t="n"/>
+      <c r="Z6" s="102" t="n"/>
       <c r="AA6" s="40" t="n"/>
-      <c r="AB6" s="94" t="inlineStr">
+      <c r="AB6" s="96" t="inlineStr">
         <is>
           <t>Use or cancellation</t>
         </is>
       </c>
-      <c r="AC6" s="103" t="n"/>
-      <c r="AD6" s="103" t="n"/>
-      <c r="AE6" s="103" t="n"/>
+      <c r="AC6" s="102" t="n"/>
+      <c r="AD6" s="102" t="n"/>
+      <c r="AE6" s="102" t="n"/>
       <c r="AF6" s="36" t="n"/>
       <c r="AG6" s="23" t="n"/>
       <c r="AH6" s="23" t="n"/>
@@ -3506,7 +3486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:U33"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="U7" sqref="U7"/>
@@ -3536,63 +3516,66 @@
     <col width="8.83203125" customWidth="1" style="15" min="22" max="16384"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n"/>
+    </row>
     <row r="3" ht="16" customHeight="1" thickBot="1">
-      <c r="B3" s="96" t="inlineStr">
+      <c r="B3" s="98" t="inlineStr">
         <is>
           <t>Table 4: Holdings</t>
         </is>
       </c>
-      <c r="C3" s="105" t="n"/>
-      <c r="D3" s="105" t="n"/>
-      <c r="E3" s="105" t="n"/>
-      <c r="F3" s="105" t="n"/>
-      <c r="G3" s="105" t="n"/>
-      <c r="H3" s="105" t="n"/>
-      <c r="I3" s="105" t="n"/>
-      <c r="J3" s="105" t="n"/>
-      <c r="K3" s="105" t="n"/>
+      <c r="C3" s="103" t="n"/>
+      <c r="D3" s="103" t="n"/>
+      <c r="E3" s="103" t="n"/>
+      <c r="F3" s="103" t="n"/>
+      <c r="G3" s="103" t="n"/>
+      <c r="H3" s="103" t="n"/>
+      <c r="I3" s="103" t="n"/>
+      <c r="J3" s="103" t="n"/>
+      <c r="K3" s="103" t="n"/>
       <c r="L3" s="50" t="n"/>
-      <c r="M3" s="97" t="n"/>
-      <c r="N3" s="105" t="n"/>
-      <c r="O3" s="105" t="n"/>
-      <c r="P3" s="105" t="n"/>
-      <c r="Q3" s="105" t="n"/>
-      <c r="R3" s="105" t="n"/>
-      <c r="S3" s="105" t="n"/>
-      <c r="T3" s="105" t="n"/>
+      <c r="M3" s="99" t="n"/>
+      <c r="N3" s="103" t="n"/>
+      <c r="O3" s="103" t="n"/>
+      <c r="P3" s="103" t="n"/>
+      <c r="Q3" s="103" t="n"/>
+      <c r="R3" s="103" t="n"/>
+      <c r="S3" s="103" t="n"/>
+      <c r="T3" s="103" t="n"/>
     </row>
     <row r="4" ht="14.5" customHeight="1">
       <c r="B4" s="66" t="n"/>
       <c r="C4" s="67" t="n"/>
       <c r="D4" s="68" t="n"/>
       <c r="E4" s="67" t="n"/>
-      <c r="F4" s="98" t="inlineStr">
+      <c r="F4" s="100" t="inlineStr">
         <is>
           <t>Unique identifiers</t>
         </is>
       </c>
-      <c r="G4" s="106" t="n"/>
-      <c r="H4" s="106" t="n"/>
-      <c r="I4" s="106" t="n"/>
-      <c r="J4" s="106" t="n"/>
-      <c r="K4" s="106" t="n"/>
+      <c r="G4" s="104" t="n"/>
+      <c r="H4" s="104" t="n"/>
+      <c r="I4" s="104" t="n"/>
+      <c r="J4" s="104" t="n"/>
+      <c r="K4" s="104" t="n"/>
       <c r="L4" s="69" t="n"/>
-      <c r="M4" s="98" t="inlineStr">
+      <c r="M4" s="100" t="inlineStr">
         <is>
           <t>Metric and quantity</t>
         </is>
       </c>
-      <c r="N4" s="106" t="n"/>
-      <c r="O4" s="106" t="n"/>
-      <c r="P4" s="106" t="n"/>
-      <c r="Q4" s="106" t="n"/>
+      <c r="N4" s="104" t="n"/>
+      <c r="O4" s="104" t="n"/>
+      <c r="P4" s="104" t="n"/>
+      <c r="Q4" s="104" t="n"/>
       <c r="R4" s="69" t="n"/>
-      <c r="S4" s="98" t="inlineStr">
+      <c r="S4" s="100" t="inlineStr">
         <is>
           <t>ITMO details</t>
         </is>
       </c>
-      <c r="T4" s="106" t="n"/>
+      <c r="T4" s="104" t="n"/>
       <c r="U4" s="36" t="n"/>
     </row>
     <row r="5" ht="14.5" customHeight="1">
@@ -3600,20 +3583,20 @@
       <c r="C5" s="23" t="n"/>
       <c r="D5" s="38" t="n"/>
       <c r="E5" s="38" t="n"/>
-      <c r="F5" s="94" t="inlineStr">
+      <c r="F5" s="96" t="inlineStr">
         <is>
           <t>ITMO unique identifier</t>
         </is>
       </c>
-      <c r="G5" s="103" t="n"/>
+      <c r="G5" s="102" t="n"/>
       <c r="H5" s="18" t="n"/>
-      <c r="I5" s="94" t="inlineStr">
+      <c r="I5" s="96" t="inlineStr">
         <is>
           <t>Underlying units</t>
         </is>
       </c>
-      <c r="J5" s="103" t="n"/>
-      <c r="K5" s="103" t="n"/>
+      <c r="J5" s="102" t="n"/>
+      <c r="K5" s="102" t="n"/>
       <c r="L5" s="18" t="n"/>
       <c r="M5" s="38" t="n"/>
       <c r="N5" s="38" t="n"/>
@@ -3634,12 +3617,12 @@
       <c r="G6" s="37" t="n"/>
       <c r="H6" s="18" t="n"/>
       <c r="I6" s="23" t="n"/>
-      <c r="J6" s="94" t="inlineStr">
+      <c r="J6" s="96" t="inlineStr">
         <is>
           <t>Underlying unit unique identifier</t>
         </is>
       </c>
-      <c r="K6" s="103" t="n"/>
+      <c r="K6" s="102" t="n"/>
       <c r="L6" s="18" t="n"/>
       <c r="M6" s="38" t="n"/>
       <c r="N6" s="38" t="n"/>
@@ -4196,14 +4179,10 @@
       <c r="T26" s="19" t="n"/>
       <c r="U26" s="19" t="n"/>
     </row>
-    <row r="27"/>
-    <row r="28"/>
     <row r="29" ht="40.25" customHeight="1"/>
-    <row r="30"/>
     <row r="31">
       <c r="B31" s="18" t="n"/>
     </row>
-    <row r="32"/>
     <row r="33" ht="34.25" customHeight="1" thickBot="1">
       <c r="B33" s="48" t="n"/>
       <c r="C33" s="48" t="n"/>
@@ -4250,7 +4229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C8:K13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
@@ -4269,6 +4248,9 @@
     <col width="9.1640625" customWidth="1" style="15" min="11" max="16384"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n"/>
+    </row>
     <row r="8" ht="20.25" customHeight="1">
       <c r="C8" s="17" t="inlineStr">
         <is>
@@ -4278,13 +4260,13 @@
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="C9" s="51" t="n"/>
-      <c r="D9" s="94" t="inlineStr">
+      <c r="D9" s="96" t="inlineStr">
         <is>
           <t>Authorized entity</t>
         </is>
       </c>
-      <c r="E9" s="103" t="n"/>
-      <c r="F9" s="103" t="n"/>
+      <c r="E9" s="102" t="n"/>
+      <c r="F9" s="102" t="n"/>
       <c r="G9" s="52" t="n"/>
       <c r="H9" s="51" t="n"/>
       <c r="I9" s="51" t="n"/>
@@ -4378,7 +4360,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4394,309 +4376,199 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Structure check</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Correct number of worksheets in workbook.</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Correct number of worksheets in workbook</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Index</t>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>All worksheets found in workbook.</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Summary information</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Summary information: Table 1: Submission</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Table 1 Submission</t>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Table 2 Authorizations</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Summary information: Table 2: Authorizations</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Table 3 Actions</t>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Table 4 Holdings</t>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Summary information: Table 3: Actions</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Table 5 Auth. entities</t>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Summary information: Table 4: Holdings</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
         <is>
-          <t>All workseets found in workbook.</t>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Summary information</t>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Table 1 Submission</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Table 1 Submission</t>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Table 2 Authorizations</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="B16" t="inlineStr">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>The field 'Authorized quantity' cannot be found in worksheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Table 3 Actions</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
+    <row r="18">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
         <is>
           <t>Table 4 Holdings</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
+    <row r="20">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Table 5 Auth. entities</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Checking the content of 'Table 1 Submission'</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" t="inlineStr">
+    <row r="22">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Version' must conform to X.Y.</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Checking the content of 'Table 2 Authorizations'</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Activity type(s)' can only contain alphanumeric, and space characters.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Purposes for authorization' must be one of 'NDC', 'OIMP', 'IMP', 'OP', 'NDC and OIMP', 'NDC and IMP', or 'NDC and OP'.</t>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>All fields found.</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Authorized Party(ies) ID' must a comma-separated list of ISO 3166 alpha-3 codes.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Authorized timeframe' must be empty of a year range (dddd - dddd)</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Checking the content of 'Table 3 Actions'</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Action date must be in the format dd/mm/yyyy</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Action type'' must be one of 'Acquistion', 'Transfer', 'Use', 'Cancellation', 'First transfer'</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Checking the content of 'Table 4 Holdings'</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'First transferring participating Party ID' must an ISO 3166 alpha-3 country code.</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Party ITMO registry ID' must be a Party ID followed by two digits</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Checking the content of 'Table 5 Auth. entities'</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Cell content error: The value provided for 'Date of the authorization must be in the format dd/mm/yyyy</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Syntax check found errors.</t>
         </is>
@@ -4704,19 +4576,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C22" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C23" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C24" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C25" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C27" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C28" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C29" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C30" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C31" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C33" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C34" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C36" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D6" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D8" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D10" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D12" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D14" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D16" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D18" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D20" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D22" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5034,17 +4902,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD914F1E-4F53-45F4-BC1E-7EF3F88A5A0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A802338C-03A7-4AF2-B82B-337D2BACA9AD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B1A0AE8-CC32-4283-A5C1-87C74821E965}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C7D61-F8D9-47D2-8A07-10AD05B0B8B1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1590130-25C9-48B8-82F8-D67A90BF65B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{738C50FE-607A-4687-91B2-A580D0FD6F5F}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5235138C-9377-42AF-9E7B-B62B08CD6318}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AC51678-07CB-4D5B-835B-3A2C0FEDD4FC}"/>
 </file>
</xml_diff>

<commit_message>
Output formatting and cleaning up code base
</commit_message>
<xml_diff>
--- a/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2021.syntax_checked.xlsx
+++ b/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2021.syntax_checked.xlsx
@@ -33,7 +33,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -195,6 +195,16 @@
       <color theme="1"/>
       <sz val="10"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <i val="1"/>
+    </font>
+    <font>
+      <color rgb="000000FF"/>
+      <u val="single"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -343,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -598,19 +608,22 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +739,7 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>The field 'Authorized quantity' cannot be found in worksheet</t>
+        <t>The field 'OIMP authorized by the Party' cannot be found in worksheet</t>
       </text>
     </comment>
   </commentList>
@@ -2431,7 +2444,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2592,7 +2605,7 @@
       </c>
       <c r="P7" s="21" t="inlineStr">
         <is>
-          <t>OIMP authorized by the Party</t>
+          <t>OIMP authorized by the Party2</t>
         </is>
       </c>
       <c r="Q7" s="21" t="inlineStr">
@@ -3520,7 +3533,7 @@
       <c r="A1" t="n"/>
     </row>
     <row r="3" ht="16" customHeight="1" thickBot="1">
-      <c r="B3" s="98" t="inlineStr">
+      <c r="B3" s="99" t="inlineStr">
         <is>
           <t>Table 4: Holdings</t>
         </is>
@@ -3535,7 +3548,7 @@
       <c r="J3" s="103" t="n"/>
       <c r="K3" s="103" t="n"/>
       <c r="L3" s="50" t="n"/>
-      <c r="M3" s="99" t="n"/>
+      <c r="M3" s="100" t="n"/>
       <c r="N3" s="103" t="n"/>
       <c r="O3" s="103" t="n"/>
       <c r="P3" s="103" t="n"/>
@@ -3549,7 +3562,7 @@
       <c r="C4" s="67" t="n"/>
       <c r="D4" s="68" t="n"/>
       <c r="E4" s="67" t="n"/>
-      <c r="F4" s="100" t="inlineStr">
+      <c r="F4" s="98" t="inlineStr">
         <is>
           <t>Unique identifiers</t>
         </is>
@@ -3560,7 +3573,7 @@
       <c r="J4" s="104" t="n"/>
       <c r="K4" s="104" t="n"/>
       <c r="L4" s="69" t="n"/>
-      <c r="M4" s="100" t="inlineStr">
+      <c r="M4" s="98" t="inlineStr">
         <is>
           <t>Metric and quantity</t>
         </is>
@@ -3570,7 +3583,7 @@
       <c r="P4" s="104" t="n"/>
       <c r="Q4" s="104" t="n"/>
       <c r="R4" s="69" t="n"/>
-      <c r="S4" s="100" t="inlineStr">
+      <c r="S4" s="98" t="inlineStr">
         <is>
           <t>ITMO details</t>
         </is>
@@ -4360,7 +4373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4369,14 +4382,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="105" t="inlineStr">
         <is>
           <t>202504292100---AEF_CMA6_second_iteration - Guyana 2021.xlsx</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="106" t="inlineStr">
         <is>
           <t>Structure check</t>
         </is>
@@ -4404,7 +4417,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -4423,7 +4436,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -4442,7 +4455,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -4461,7 +4474,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -4480,7 +4493,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -4499,7 +4512,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -4511,64 +4524,76 @@
       </c>
     </row>
     <row r="17">
-      <c r="C17" t="inlineStr">
+      <c r="D17" s="107" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>The field 'OIMP authorized by the Party' cannot be found in worksheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Table 3 Actions</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="D18" t="inlineStr">
+    <row r="19">
+      <c r="D19" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>All fields found.</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="C19" t="inlineStr">
+    <row r="20">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Table 4 Holdings</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="D20" t="inlineStr">
+    <row r="21">
+      <c r="D21" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>All fields found.</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="C21" t="inlineStr">
+    <row r="22">
+      <c r="C22" t="inlineStr">
         <is>
           <t>Table 5 Auth. entities</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="D22" t="inlineStr">
+    <row r="23">
+      <c r="D23" s="107" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>All fields found.</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="25">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Syntax check found errors.</t>
         </is>
@@ -4582,9 +4607,10 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D12" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D14" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D16" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D18" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D20" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D22" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D17" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D19" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D21" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D23" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4902,17 +4928,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A802338C-03A7-4AF2-B82B-337D2BACA9AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A67B88B-FCC1-4C43-8571-4D1BEF7ED35F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C7D61-F8D9-47D2-8A07-10AD05B0B8B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350FDBB7-ECC8-4949-97D2-267AFE0FDB4C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{738C50FE-607A-4687-91B2-A580D0FD6F5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF23B17F-7EB4-4DA6-933A-D69EDEB6BD4C}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AC51678-07CB-4D5B-835B-3A2C0FEDD4FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B915A36-4BBA-4FD6-95CF-2896C0995F0D}"/>
 </file>
</xml_diff>